<commit_message>
sammy is a butt
</commit_message>
<xml_diff>
--- a/nhl_shots_data_2021.xlsx
+++ b/nhl_shots_data_2021.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,35 +498,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021020001</t>
+          <t>2021020003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Amalie Arena</t>
+          <t>Scotiabank Arena</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>40.0 meters meters</t>
+          <t>86.0 meters meters</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>October 12, 2021</t>
+          <t>October 13, 2021</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pittsburgh Penguins vs. Tampa Bay Lightning</t>
+          <t>Montreal Canadiens (0-0-0) vs. Toronto Maple Leafs (0-0-0)</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>00:04</t>
+          <t>00:03</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -536,140 +536,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Brian Dumoulin (Penguins)</t>
+          <t>Jeff Petry (Canadiens)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>64.88 feet</t>
+          <t>23.41 feet</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2 - 0</t>
+          <t>1 - 2</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
-        <is>
-          <t>https://www.nhl.com/scores/htmlreports/20212022/PL020001.HTM</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021020001</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Amalie Arena</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>40.0 meters meters</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>October 12, 2021</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Pittsburgh Penguins vs. Tampa Bay Lightning</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>00:05</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>SHOT</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Erik Cernak (Lightning)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>59.06 feet</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>6 - 2</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>https://www.nhl.com/scores/htmlreports/20212022/PL020001.HTM</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021020003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Scotiabank Arena</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>86.0 meters meters</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>October 13, 2021</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Montreal Canadiens vs. Toronto Maple Leafs</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>00:03</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>SHOT</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Jeff Petry (Canadiens)</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>23.41 feet</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1 - 2</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
         <is>
           <t>https://www.nhl.com/scores/htmlreports/20212022/PL020003.HTM</t>
         </is>

</xml_diff>